<commit_message>
add : google OR toolsを導入
</commit_message>
<xml_diff>
--- a/backend/食品標準成分表示_主食・肉類.xlsx
+++ b/backend/食品標準成分表示_主食・肉類.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\81809\OneDrive - 名古屋市立大学\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1F7446-B356-4268-BDA9-50B6F65ECB84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8479F6D1-B309-4AB1-B910-CBAE7F2BF3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{7E36C7B1-DE88-404E-95FC-DCA1FB1238F9}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="99">
   <si>
     <t>可　　食　　部　　 100　　g　　当　　た　　り</t>
   </si>
@@ -839,19 +839,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="double">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -861,26 +848,6 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -927,28 +894,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1007,6 +952,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1014,7 +1016,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1063,7 +1065,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1105,14 +1107,47 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1132,62 +1167,38 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1524,10 +1535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53B3E39-95ED-4142-9E14-53CE5E556F6C}">
-  <dimension ref="A1:AB32"/>
+  <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="X18" sqref="X18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="75" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -1621,16 +1632,16 @@
       <c r="R2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="S2" s="15" t="s">
+      <c r="S2" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="T2" s="15" t="s">
+      <c r="T2" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="U2" s="15" t="s">
+      <c r="U2" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="V2" s="16" t="s">
+      <c r="V2" s="60" t="s">
         <v>27</v>
       </c>
       <c r="W2" s="17" t="s">
@@ -1663,44 +1674,44 @@
       <c r="D3" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35" t="s">
+      <c r="F3" s="45"/>
+      <c r="G3" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="35" t="s">
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="M3" s="37"/>
-      <c r="N3" s="33" t="s">
+      <c r="M3" s="48"/>
+      <c r="N3" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="O3" s="38"/>
-      <c r="P3" s="34"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="45"/>
       <c r="Q3" s="24" t="s">
         <v>38</v>
       </c>
       <c r="R3" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="S3" s="30" t="s">
+      <c r="S3" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="T3" s="31"/>
-      <c r="U3" s="31"/>
-      <c r="V3" s="32"/>
-      <c r="W3" s="52"/>
-      <c r="X3" s="53"/>
-      <c r="Y3" s="53"/>
-      <c r="Z3" s="53"/>
-      <c r="AA3" s="53"/>
-      <c r="AB3" s="54"/>
+      <c r="T3" s="47"/>
+      <c r="U3" s="47"/>
+      <c r="V3" s="57"/>
+      <c r="W3" s="36"/>
+      <c r="X3" s="36"/>
+      <c r="Y3" s="36"/>
+      <c r="Z3" s="36"/>
+      <c r="AA3" s="36"/>
+      <c r="AB3" s="37"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="26" t="s">
@@ -1766,7 +1777,7 @@
       <c r="U4" s="1">
         <v>145.875</v>
       </c>
-      <c r="V4" s="40">
+      <c r="V4" s="54">
         <v>155.67500000000001</v>
       </c>
       <c r="W4" s="1">
@@ -1784,7 +1795,7 @@
       <c r="AA4" s="1">
         <v>68.037499999999994</v>
       </c>
-      <c r="AB4" s="55">
+      <c r="AB4" s="38">
         <v>44.686249999999987</v>
       </c>
     </row>
@@ -1852,7 +1863,7 @@
       <c r="U5" s="1">
         <v>82.85</v>
       </c>
-      <c r="V5" s="41">
+      <c r="V5" s="54">
         <v>94.75</v>
       </c>
       <c r="W5" s="1">
@@ -1870,7 +1881,7 @@
       <c r="AA5" s="1">
         <v>35.474999999999994</v>
       </c>
-      <c r="AB5" s="56">
+      <c r="AB5" s="39">
         <v>21.262499999999996</v>
       </c>
     </row>
@@ -1938,7 +1949,7 @@
       <c r="U6" s="1">
         <v>123.375</v>
       </c>
-      <c r="V6" s="41">
+      <c r="V6" s="54">
         <v>150.875</v>
       </c>
       <c r="W6" s="1">
@@ -1956,7 +1967,7 @@
       <c r="AA6" s="1">
         <v>47.9375</v>
       </c>
-      <c r="AB6" s="56">
+      <c r="AB6" s="39">
         <v>25.306249999999991</v>
       </c>
     </row>
@@ -2024,7 +2035,7 @@
       <c r="U7" s="1">
         <v>132.67999999999998</v>
       </c>
-      <c r="V7" s="41">
+      <c r="V7" s="54">
         <v>164.97999999999996</v>
       </c>
       <c r="W7" s="1">
@@ -2042,7 +2053,7 @@
       <c r="AA7" s="1">
         <v>50.19</v>
       </c>
-      <c r="AB7" s="56">
+      <c r="AB7" s="39">
         <v>25.442999999999998</v>
       </c>
     </row>
@@ -2110,7 +2121,7 @@
       <c r="U8" s="1">
         <v>1.125</v>
       </c>
-      <c r="V8" s="41">
+      <c r="V8" s="54">
         <v>231.52500000000001</v>
       </c>
       <c r="W8" s="1">
@@ -2128,7 +2139,7 @@
       <c r="AA8" s="1">
         <v>-114.6375</v>
       </c>
-      <c r="AB8" s="56">
+      <c r="AB8" s="39">
         <v>-149.36625000000001</v>
       </c>
     </row>
@@ -2196,7 +2207,7 @@
       <c r="U9" s="1">
         <v>16.5</v>
       </c>
-      <c r="V9" s="41">
+      <c r="V9" s="54">
         <v>293.59999999999997</v>
       </c>
       <c r="W9" s="1">
@@ -2214,7 +2225,7 @@
       <c r="AA9" s="1">
         <v>-130.29999999999998</v>
       </c>
-      <c r="AB9" s="56">
+      <c r="AB9" s="39">
         <v>-174.33999999999997</v>
       </c>
     </row>
@@ -2282,7 +2293,7 @@
       <c r="U10" s="1">
         <v>14.625</v>
       </c>
-      <c r="V10" s="41">
+      <c r="V10" s="54">
         <v>379.625</v>
       </c>
       <c r="W10" s="1">
@@ -2300,7 +2311,7 @@
       <c r="AA10" s="1">
         <v>-175.1875</v>
       </c>
-      <c r="AB10" s="56">
+      <c r="AB10" s="39">
         <v>-232.13124999999999</v>
       </c>
     </row>
@@ -2368,7 +2379,7 @@
       <c r="U11" s="1">
         <v>15.374999999999998</v>
       </c>
-      <c r="V11" s="41">
+      <c r="V11" s="54">
         <v>311.67499999999995</v>
       </c>
       <c r="W11" s="1">
@@ -2386,7 +2397,7 @@
       <c r="AA11" s="1">
         <v>-140.46249999999998</v>
       </c>
-      <c r="AB11" s="56">
+      <c r="AB11" s="39">
         <v>-187.21374999999998</v>
       </c>
     </row>
@@ -2454,7 +2465,7 @@
       <c r="U12" s="1">
         <v>1.125</v>
       </c>
-      <c r="V12" s="41">
+      <c r="V12" s="54">
         <v>381.22499999999997</v>
       </c>
       <c r="W12" s="1">
@@ -2472,7 +2483,7 @@
       <c r="AA12" s="1">
         <v>-189.48749999999998</v>
       </c>
-      <c r="AB12" s="56">
+      <c r="AB12" s="39">
         <v>-246.67124999999999</v>
       </c>
     </row>
@@ -2540,7 +2551,7 @@
       <c r="U13" s="1">
         <v>17.25</v>
       </c>
-      <c r="V13" s="41">
+      <c r="V13" s="54">
         <v>194.64999999999998</v>
       </c>
       <c r="W13" s="1">
@@ -2558,7 +2569,7 @@
       <c r="AA13" s="1">
         <v>-80.074999999999989</v>
       </c>
-      <c r="AB13" s="56">
+      <c r="AB13" s="39">
         <v>-109.27249999999999</v>
       </c>
     </row>
@@ -2626,7 +2637,7 @@
       <c r="U14" s="1">
         <v>15.75</v>
       </c>
-      <c r="V14" s="41">
+      <c r="V14" s="54">
         <v>218.85</v>
       </c>
       <c r="W14" s="1">
@@ -2644,7 +2655,7 @@
       <c r="AA14" s="1">
         <v>-93.674999999999997</v>
       </c>
-      <c r="AB14" s="56">
+      <c r="AB14" s="39">
         <v>-126.5025</v>
       </c>
     </row>
@@ -2712,7 +2723,7 @@
       <c r="U15" s="1">
         <v>17.25</v>
       </c>
-      <c r="V15" s="41">
+      <c r="V15" s="54">
         <v>232.35000000000002</v>
       </c>
       <c r="W15" s="1">
@@ -2730,7 +2741,7 @@
       <c r="AA15" s="1">
         <v>-98.925000000000011</v>
       </c>
-      <c r="AB15" s="56">
+      <c r="AB15" s="39">
         <v>-133.77750000000003</v>
       </c>
     </row>
@@ -2798,7 +2809,7 @@
       <c r="U16" s="1">
         <v>14.25</v>
       </c>
-      <c r="V16" s="41">
+      <c r="V16" s="54">
         <v>175.95</v>
       </c>
       <c r="W16" s="1">
@@ -2816,7 +2827,7 @@
       <c r="AA16" s="1">
         <v>-73.724999999999994</v>
       </c>
-      <c r="AB16" s="56">
+      <c r="AB16" s="39">
         <v>-100.11749999999999</v>
       </c>
     </row>
@@ -2884,7 +2895,7 @@
       <c r="U17" s="1">
         <v>0.75</v>
       </c>
-      <c r="V17" s="41">
+      <c r="V17" s="54">
         <v>200.75</v>
       </c>
       <c r="W17" s="1">
@@ -2902,7 +2913,7 @@
       <c r="AA17" s="1">
         <v>-99.625</v>
       </c>
-      <c r="AB17" s="56">
+      <c r="AB17" s="39">
         <v>-129.73750000000001</v>
       </c>
     </row>
@@ -2970,7 +2981,7 @@
       <c r="U18" s="1">
         <v>12.75</v>
       </c>
-      <c r="V18" s="41">
+      <c r="V18" s="54">
         <v>237.14999999999998</v>
       </c>
       <c r="W18" s="1">
@@ -2988,7 +2999,7 @@
       <c r="AA18" s="1">
         <v>-105.82499999999999</v>
       </c>
-      <c r="AB18" s="56">
+      <c r="AB18" s="39">
         <v>-141.39749999999998</v>
       </c>
     </row>
@@ -3056,7 +3067,7 @@
       <c r="U19" s="1">
         <v>11.25</v>
       </c>
-      <c r="V19" s="41">
+      <c r="V19" s="54">
         <v>246.55</v>
       </c>
       <c r="W19" s="1">
@@ -3074,7 +3085,7 @@
       <c r="AA19" s="1">
         <v>-112.02500000000001</v>
       </c>
-      <c r="AB19" s="56">
+      <c r="AB19" s="39">
         <v>-149.00750000000002</v>
       </c>
     </row>
@@ -3142,7 +3153,7 @@
       <c r="U20" s="1">
         <v>0.375</v>
       </c>
-      <c r="V20" s="41">
+      <c r="V20" s="54">
         <v>365.67499999999995</v>
       </c>
       <c r="W20" s="1">
@@ -3160,7 +3171,7 @@
       <c r="AA20" s="1">
         <v>-182.46249999999998</v>
       </c>
-      <c r="AB20" s="56">
+      <c r="AB20" s="39">
         <v>-237.31374999999997</v>
       </c>
     </row>
@@ -3228,7 +3239,7 @@
       <c r="U21" s="1">
         <v>17.25</v>
       </c>
-      <c r="V21" s="41">
+      <c r="V21" s="54">
         <v>170.35</v>
       </c>
       <c r="W21" s="1">
@@ -3246,7 +3257,7 @@
       <c r="AA21" s="1">
         <v>-67.924999999999997</v>
       </c>
-      <c r="AB21" s="56">
+      <c r="AB21" s="39">
         <v>-93.477500000000006</v>
       </c>
     </row>
@@ -3314,7 +3325,7 @@
       <c r="U22" s="1">
         <v>15</v>
       </c>
-      <c r="V22" s="41">
+      <c r="V22" s="54">
         <v>220.5</v>
       </c>
       <c r="W22" s="1">
@@ -3332,7 +3343,7 @@
       <c r="AA22" s="1">
         <v>-95.25</v>
       </c>
-      <c r="AB22" s="56">
+      <c r="AB22" s="39">
         <v>-128.32500000000002</v>
       </c>
     </row>
@@ -3400,7 +3411,7 @@
       <c r="U23" s="1">
         <v>13.875</v>
       </c>
-      <c r="V23" s="41">
+      <c r="V23" s="54">
         <v>117.575</v>
       </c>
       <c r="W23" s="1">
@@ -3418,7 +3429,7 @@
       <c r="AA23" s="1">
         <v>-44.912500000000001</v>
       </c>
-      <c r="AB23" s="56">
+      <c r="AB23" s="39">
         <v>-62.548749999999998</v>
       </c>
     </row>
@@ -3486,7 +3497,7 @@
       <c r="U24" s="1">
         <v>0</v>
       </c>
-      <c r="V24" s="41">
+      <c r="V24" s="54">
         <v>189.3</v>
       </c>
       <c r="W24" s="1">
@@ -3504,7 +3515,7 @@
       <c r="AA24" s="1">
         <v>-94.65</v>
       </c>
-      <c r="AB24" s="56">
+      <c r="AB24" s="39">
         <v>-123.04500000000002</v>
       </c>
     </row>
@@ -3572,7 +3583,7 @@
       <c r="U25" s="1">
         <v>0</v>
       </c>
-      <c r="V25" s="41">
+      <c r="V25" s="54">
         <v>206.5</v>
       </c>
       <c r="W25" s="1">
@@ -3590,7 +3601,7 @@
       <c r="AA25" s="1">
         <v>-103.25</v>
       </c>
-      <c r="AB25" s="56">
+      <c r="AB25" s="39">
         <v>-134.22499999999999</v>
       </c>
     </row>
@@ -3658,7 +3669,7 @@
       <c r="U26" s="1">
         <v>0</v>
       </c>
-      <c r="V26" s="41">
+      <c r="V26" s="54">
         <v>175.7</v>
       </c>
       <c r="W26" s="1">
@@ -3676,7 +3687,7 @@
       <c r="AA26" s="1">
         <v>-87.85</v>
       </c>
-      <c r="AB26" s="56">
+      <c r="AB26" s="39">
         <v>-114.205</v>
       </c>
     </row>
@@ -3744,7 +3755,7 @@
       <c r="U27" s="1">
         <v>13.5</v>
       </c>
-      <c r="V27" s="41">
+      <c r="V27" s="54">
         <v>132.19999999999999</v>
       </c>
       <c r="W27" s="1">
@@ -3762,7 +3773,7 @@
       <c r="AA27" s="1">
         <v>-52.599999999999994</v>
       </c>
-      <c r="AB27" s="56">
+      <c r="AB27" s="39">
         <v>-72.429999999999993</v>
       </c>
     </row>
@@ -3830,7 +3841,7 @@
       <c r="U28" s="1">
         <v>0</v>
       </c>
-      <c r="V28" s="41">
+      <c r="V28" s="54">
         <v>189.5</v>
       </c>
       <c r="W28" s="1">
@@ -3848,7 +3859,7 @@
       <c r="AA28" s="1">
         <v>-94.75</v>
       </c>
-      <c r="AB28" s="56">
+      <c r="AB28" s="39">
         <v>-123.175</v>
       </c>
     </row>
@@ -3916,7 +3927,7 @@
       <c r="U29" s="1">
         <v>12.6</v>
       </c>
-      <c r="V29" s="41">
+      <c r="V29" s="54">
         <v>95.899999999999991</v>
       </c>
       <c r="W29" s="1">
@@ -3934,203 +3945,94 @@
       <c r="AA29" s="1">
         <v>-35.349999999999994</v>
       </c>
-      <c r="AB29" s="56">
+      <c r="AB29" s="39">
         <v>-49.734999999999992</v>
       </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="B30" s="26">
+      <c r="B30" s="41">
         <v>100</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="42">
         <v>134</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E30" s="42">
         <v>14.6</v>
       </c>
-      <c r="F30" s="1">
-        <v>0</v>
-      </c>
-      <c r="G30" s="1">
+      <c r="F30" s="42">
+        <v>0</v>
+      </c>
+      <c r="G30" s="42">
         <v>250</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H30" s="42">
         <v>8</v>
       </c>
-      <c r="I30" s="1">
+      <c r="I30" s="42">
         <v>24</v>
       </c>
-      <c r="J30" s="1">
+      <c r="J30" s="42">
         <v>0.8</v>
       </c>
-      <c r="K30" s="1">
+      <c r="K30" s="42">
         <v>1.1000000000000001</v>
       </c>
-      <c r="L30" s="1">
+      <c r="L30" s="42">
         <v>37</v>
       </c>
-      <c r="M30" s="1">
+      <c r="M30" s="42">
         <v>0.1</v>
       </c>
-      <c r="N30" s="1">
+      <c r="N30" s="42">
         <v>0.09</v>
       </c>
-      <c r="O30" s="1">
+      <c r="O30" s="42">
         <v>0.17</v>
       </c>
-      <c r="P30" s="1">
+      <c r="P30" s="42">
         <v>0.52</v>
       </c>
-      <c r="Q30" s="1">
+      <c r="Q30" s="42">
         <v>10</v>
       </c>
-      <c r="R30" s="27">
+      <c r="R30" s="43">
         <v>1</v>
       </c>
-      <c r="S30" s="1">
+      <c r="S30" s="53">
         <v>58.4</v>
       </c>
-      <c r="T30" s="1">
+      <c r="T30" s="42">
         <v>99</v>
       </c>
-      <c r="U30" s="1">
+      <c r="U30" s="42">
         <v>12.75</v>
       </c>
-      <c r="V30" s="41">
+      <c r="V30" s="55">
         <v>170.15</v>
       </c>
-      <c r="W30" s="1">
+      <c r="W30" s="42">
         <v>36.280499999999996</v>
       </c>
-      <c r="X30" s="1">
+      <c r="X30" s="42">
         <v>24.369999999999997</v>
       </c>
-      <c r="Y30" s="1">
+      <c r="Y30" s="42">
         <v>64.97</v>
       </c>
-      <c r="Z30" s="1">
+      <c r="Z30" s="42">
         <v>47.954999999999998</v>
       </c>
-      <c r="AA30" s="1">
+      <c r="AA30" s="42">
         <v>-72.325000000000003</v>
       </c>
-      <c r="AB30" s="57">
+      <c r="AB30" s="40">
         <v>-97.847500000000011</v>
-      </c>
-    </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="48"/>
-      <c r="B31" s="48"/>
-      <c r="C31" s="49"/>
-      <c r="D31" s="50" t="s">
-        <v>95</v>
-      </c>
-      <c r="E31" s="49">
-        <v>65</v>
-      </c>
-      <c r="F31" s="51">
-        <v>20</v>
-      </c>
-      <c r="G31" s="51">
-        <v>2500</v>
-      </c>
-      <c r="H31" s="51">
-        <v>800</v>
-      </c>
-      <c r="I31" s="51">
-        <v>340</v>
-      </c>
-      <c r="J31" s="51">
-        <v>7.5</v>
-      </c>
-      <c r="K31" s="51">
-        <v>11</v>
-      </c>
-      <c r="L31" s="51">
-        <v>850</v>
-      </c>
-      <c r="M31" s="51">
-        <v>9</v>
-      </c>
-      <c r="N31" s="51">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="O31" s="51">
-        <v>1.6</v>
-      </c>
-      <c r="P31" s="51">
-        <v>1.5</v>
-      </c>
-      <c r="Q31" s="51">
-        <v>240</v>
-      </c>
-      <c r="R31" s="51">
-        <v>100</v>
-      </c>
-      <c r="S31" s="49"/>
-      <c r="T31" s="49"/>
-      <c r="U31" s="49"/>
-      <c r="V31" s="49"/>
-      <c r="W31" s="49"/>
-      <c r="X31" s="49"/>
-      <c r="Y31" s="49"/>
-      <c r="Z31" s="49"/>
-      <c r="AA31" s="49"/>
-      <c r="AB31" s="49"/>
-    </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="26"/>
-      <c r="B32" s="26"/>
-      <c r="D32" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="E32" s="1">
-        <v>21.67</v>
-      </c>
-      <c r="F32" s="1">
-        <v>6.67</v>
-      </c>
-      <c r="G32" s="1">
-        <v>833.33</v>
-      </c>
-      <c r="H32" s="1">
-        <v>266.67</v>
-      </c>
-      <c r="I32" s="1">
-        <v>113.33</v>
-      </c>
-      <c r="J32" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="K32" s="1">
-        <v>3.67</v>
-      </c>
-      <c r="L32" s="1">
-        <v>283.33</v>
-      </c>
-      <c r="M32" s="1">
-        <v>3</v>
-      </c>
-      <c r="N32" s="1">
-        <v>0.37</v>
-      </c>
-      <c r="O32" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="P32" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="Q32" s="1">
-        <v>80</v>
-      </c>
-      <c r="R32" s="1">
-        <v>33.33</v>
       </c>
     </row>
   </sheetData>
@@ -4150,8 +4052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8435D20D-942F-455A-B057-2DD8C4A2B19D}">
   <dimension ref="A1:AI32"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="AD3" sqref="AD3"/>
+    <sheetView topLeftCell="G2" zoomScale="75" workbookViewId="0">
+      <selection activeCell="Z1" sqref="Z1:AC30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -4288,22 +4190,22 @@
       <c r="AC2" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="AD2" s="42" t="s">
+      <c r="AD2" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="AE2" s="43" t="s">
+      <c r="AE2" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="AF2" s="44" t="s">
+      <c r="AF2" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="44" t="s">
+      <c r="AG2" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="44" t="s">
+      <c r="AH2" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="AI2" s="45" t="s">
+      <c r="AI2" s="33" t="s">
         <v>33</v>
       </c>
     </row>
@@ -4318,53 +4220,53 @@
       <c r="D3" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35" t="s">
+      <c r="F3" s="45"/>
+      <c r="G3" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="35" t="s">
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="M3" s="37"/>
-      <c r="N3" s="33" t="s">
+      <c r="M3" s="48"/>
+      <c r="N3" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="O3" s="38"/>
-      <c r="P3" s="34"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="45"/>
       <c r="Q3" s="24" t="s">
         <v>38</v>
       </c>
       <c r="R3" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="S3" s="39" t="s">
+      <c r="S3" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="T3" s="39"/>
-      <c r="U3" s="39"/>
-      <c r="V3" s="39"/>
-      <c r="W3" s="39"/>
-      <c r="X3" s="39"/>
-      <c r="Y3" s="39"/>
-      <c r="Z3" s="30" t="s">
+      <c r="T3" s="52"/>
+      <c r="U3" s="52"/>
+      <c r="V3" s="52"/>
+      <c r="W3" s="52"/>
+      <c r="X3" s="52"/>
+      <c r="Y3" s="52"/>
+      <c r="Z3" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="AA3" s="31"/>
-      <c r="AB3" s="31"/>
-      <c r="AC3" s="31"/>
-      <c r="AD3" s="47"/>
+      <c r="AA3" s="51"/>
+      <c r="AB3" s="51"/>
+      <c r="AC3" s="51"/>
+      <c r="AD3" s="35"/>
       <c r="AE3" s="21"/>
       <c r="AF3" s="21"/>
       <c r="AG3" s="21"/>
       <c r="AH3" s="21"/>
-      <c r="AI3" s="46"/>
+      <c r="AI3" s="34"/>
     </row>
     <row r="4" spans="1:35" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="26" t="s">

</xml_diff>